<commit_message>
Added Code for 1) WIP-LUI_Work Complete Flow 2)VF-System Setup_Pragati's Testcases
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/Create Engineering Item Master.xlsx
+++ b/templates/AutomationOrg/Create Engineering Item Master.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="143">
   <si>
     <t>Item Number</t>
   </si>
@@ -433,6 +433,42 @@
   </si>
   <si>
     <t>a345f000000uI3IAAU</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-RV982</t>
+  </si>
+  <si>
+    <t>a345f000000uQ1FAAU</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-SWEOX</t>
+  </si>
+  <si>
+    <t>a345f000000uQ1KAAU</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-UN0SV</t>
+  </si>
+  <si>
+    <t>a345f000000uQ1PAAU</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-FNKFK</t>
+  </si>
+  <si>
+    <t>a345f000000uRAdAAM</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-H4W3L</t>
+  </si>
+  <si>
+    <t>a345f000000uRCtAAM</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-I3FR5</t>
+  </si>
+  <si>
+    <t>a345f000000uRE6AAM</t>
   </si>
 </sst>
 </file>
@@ -443,7 +479,7 @@
     <numFmt numFmtId="164" formatCode="mm\/dd\/yyyy"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -471,6 +507,78 @@
       <color rgb="FF202124"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -553,7 +661,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -579,11 +687,29 @@
     <border>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="29">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
@@ -599,8 +725,20 @@
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="4" fillId="0" fontId="11" numFmtId="49" xfId="0"/>
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="12" numFmtId="165" xfId="0"/>
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="5" fillId="0" fontId="13" numFmtId="49" xfId="0"/>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="6" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="14" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="6" fillId="0" fontId="15" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="16" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="7" fillId="0" fontId="17" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="18" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="8" fillId="0" fontId="19" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="20" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="9" fillId="0" fontId="21" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="22" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="10" fillId="0" fontId="23" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="24" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="11" fillId="0" fontId="25" numFmtId="49" xfId="0"/>
+    <xf numFmtId="165" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="27" fillId="0" borderId="12" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -1035,9 +1173,9 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.99609375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.7890625" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="20.1328125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="21.76171875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -1059,13 +1197,13 @@
         <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="C2" t="s">
         <v>117</v>
       </c>
       <c r="D2" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes in Work Order/System Setup
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/Create Engineering Item Master.xlsx
+++ b/templates/AutomationOrg/Create Engineering Item Master.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="173">
   <si>
     <t>Item Number</t>
   </si>
@@ -469,6 +469,96 @@
   </si>
   <si>
     <t>a345f000000uRE6AAM</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-7GCB2</t>
+  </si>
+  <si>
+    <t>a345f000000uT1eAAE</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-GQPN8</t>
+  </si>
+  <si>
+    <t>a345f000000uTAHAA2</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-HVRTM</t>
+  </si>
+  <si>
+    <t>a345f000000uTAMAA2</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-IXH8Q</t>
+  </si>
+  <si>
+    <t>a345f000000uTARAA2</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-IXNNL</t>
+  </si>
+  <si>
+    <t>a345f000000uTAWAA2</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-22M4L</t>
+  </si>
+  <si>
+    <t>a345f000000uTDuAAM</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-3HPWN</t>
+  </si>
+  <si>
+    <t>a345f000000uTE4AAM</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-4H23J</t>
+  </si>
+  <si>
+    <t>a345f000000uTE9AAM</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-EVRTZ</t>
+  </si>
+  <si>
+    <t>a345f000000uTO9AAM</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-FNSL5</t>
+  </si>
+  <si>
+    <t>a345f000000uTOEAA2</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-G0VZ5</t>
+  </si>
+  <si>
+    <t>a345f000000uTOJAA2</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-GX9HR</t>
+  </si>
+  <si>
+    <t>a345f000000uTOOAA2</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-03LCC</t>
+  </si>
+  <si>
+    <t>a345f000000uTa5AAE</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-J1BD0</t>
+  </si>
+  <si>
+    <t>a345f000000uTiOAAU</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-J7232</t>
+  </si>
+  <si>
+    <t>a345f000000uTj2AAE</t>
   </si>
 </sst>
 </file>
@@ -479,7 +569,7 @@
     <numFmt numFmtId="164" formatCode="mm\/dd\/yyyy"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="58" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -507,6 +597,186 @@
       <color rgb="FF202124"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -661,7 +931,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -705,11 +975,56 @@
     <border>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="59">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
@@ -737,8 +1052,38 @@
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="10" fillId="0" fontId="23" numFmtId="49" xfId="0"/>
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="24" numFmtId="165" xfId="0"/>
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="11" fillId="0" fontId="25" numFmtId="49" xfId="0"/>
-    <xf numFmtId="165" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="27" fillId="0" borderId="12" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="26" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="12" fillId="0" fontId="27" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="28" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="13" fillId="0" fontId="29" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="30" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="14" fillId="0" fontId="31" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="32" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="15" fillId="0" fontId="33" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="34" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="16" fillId="0" fontId="35" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="36" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="17" fillId="0" fontId="37" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="38" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="18" fillId="0" fontId="39" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="40" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="19" fillId="0" fontId="41" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="42" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="20" fillId="0" fontId="43" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="44" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="21" fillId="0" fontId="45" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="46" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="22" fillId="0" fontId="47" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="48" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="23" fillId="0" fontId="49" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="50" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="24" fillId="0" fontId="51" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="52" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="25" fillId="0" fontId="53" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="54" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="26" fillId="0" fontId="55" numFmtId="49" xfId="0"/>
+    <xf numFmtId="165" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="57" fillId="0" borderId="27" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -1173,9 +1518,9 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.7890625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.9609375" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="21.76171875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -1197,13 +1542,13 @@
         <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="C2" t="s">
         <v>117</v>
       </c>
       <c r="D2" t="s">
-        <v>142</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixes for WO and CPQ
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/Create Engineering Item Master.xlsx
+++ b/templates/AutomationOrg/Create Engineering Item Master.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="179">
   <si>
     <t>Item Number</t>
   </si>
@@ -559,6 +559,24 @@
   </si>
   <si>
     <t>a345f000000uTj2AAE</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-T7THO</t>
+  </si>
+  <si>
+    <t>a345f000000uUDjAAM</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-WH3TE</t>
+  </si>
+  <si>
+    <t>a345f000000uUFBAA2</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-F951G</t>
+  </si>
+  <si>
+    <t>a345f000000uUJmAAM</t>
   </si>
 </sst>
 </file>
@@ -569,7 +587,7 @@
     <numFmt numFmtId="164" formatCode="mm\/dd\/yyyy"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="58" x14ac:knownFonts="1">
+  <fonts count="64" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -597,6 +615,42 @@
       <color rgb="FF202124"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -931,7 +985,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -1020,11 +1074,20 @@
     <border>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="65">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
@@ -1082,8 +1145,14 @@
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="25" fillId="0" fontId="53" numFmtId="49" xfId="0"/>
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="54" numFmtId="165" xfId="0"/>
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="26" fillId="0" fontId="55" numFmtId="49" xfId="0"/>
-    <xf numFmtId="165" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="57" fillId="0" borderId="27" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="56" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="27" fillId="0" fontId="57" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="58" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="28" fillId="0" fontId="59" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="60" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="29" fillId="0" fontId="61" numFmtId="49" xfId="0"/>
+    <xf numFmtId="165" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="63" fillId="0" borderId="30" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -1518,9 +1587,9 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.9609375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.54296875" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="22.25" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -1542,13 +1611,13 @@
         <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="C2" t="s">
         <v>117</v>
       </c>
       <c r="D2" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>